<commit_message>
Added comments and a second controller to the test hierarchy in the main()
</commit_message>
<xml_diff>
--- a/data/base-controller.xlsx
+++ b/data/base-controller.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
   <si>
     <t>elapsed-time</t>
   </si>
@@ -25,6 +25,12 @@
     <t>RSP_parent-controller_to_board-monitor</t>
   </si>
   <si>
+    <t>CMD_parent-controller_to_child_controller</t>
+  </si>
+  <si>
+    <t>RSP_child_controller_to_parent-controller</t>
+  </si>
+  <si>
     <t>INIT</t>
   </si>
   <si>
@@ -34,10 +40,10 @@
     <t>EXECUTING</t>
   </si>
   <si>
+    <t>DONE</t>
+  </si>
+  <si>
     <t>RUN</t>
-  </si>
-  <si>
-    <t>DONE</t>
   </si>
   <si>
     <t>TERMINATE</t>
@@ -398,13 +404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:13">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -441,17 +447,8 @@
       <c r="M1" s="1">
         <v>11</v>
       </c>
-      <c r="N1" s="1">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,114 +488,169 @@
       <c r="M2">
         <v>1.2</v>
       </c>
-      <c r="N2">
-        <v>1.3</v>
-      </c>
-      <c r="O2">
-        <v>1.4</v>
-      </c>
-      <c r="P2">
-        <v>1.5</v>
-      </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" t="s">
-        <v>5</v>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>